<commit_message>
tmp save after add db init data
</commit_message>
<xml_diff>
--- a/tools/initData.xlsx
+++ b/tools/initData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="0" windowWidth="25500" windowHeight="28320" tabRatio="500"/>
+    <workbookView xWindow="4360" yWindow="0" windowWidth="25500" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="309">
   <si>
     <t>// 品牌</t>
   </si>
@@ -132,12 +132,6 @@
     <t>柜台BA</t>
   </si>
   <si>
-    <t>GTBA1</t>
-  </si>
-  <si>
-    <t>GTBA2</t>
-  </si>
-  <si>
     <t>供应商管理员</t>
   </si>
   <si>
@@ -259,24 +253,6 @@
     <t>GZ8</t>
   </si>
   <si>
-    <t>GTBA3</t>
-  </si>
-  <si>
-    <t>GTBA4</t>
-  </si>
-  <si>
-    <t>GTBA5</t>
-  </si>
-  <si>
-    <t>GTBA6</t>
-  </si>
-  <si>
-    <t>GTBA7</t>
-  </si>
-  <si>
-    <t>GTBA8</t>
-  </si>
-  <si>
     <t>GYSGLY3</t>
   </si>
   <si>
@@ -361,6 +337,708 @@
   </si>
   <si>
     <t>安装公司管理员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[GT]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT1Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT1BA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT2BA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT3BA</t>
+  </si>
+  <si>
+    <t>GT4BA</t>
+  </si>
+  <si>
+    <t>GT5BA</t>
+  </si>
+  <si>
+    <t>GT6BA</t>
+  </si>
+  <si>
+    <t>GT7BA</t>
+  </si>
+  <si>
+    <t>GT8BA</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>QY</t>
+  </si>
+  <si>
+    <t>GTBAUserId</t>
+  </si>
+  <si>
+    <t>GZUserId</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>imageUrl</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上海</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>广州</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>南区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT2Code</t>
+  </si>
+  <si>
+    <t>GT3Code</t>
+  </si>
+  <si>
+    <t>GT4Code</t>
+  </si>
+  <si>
+    <t>GT5Code</t>
+  </si>
+  <si>
+    <t>GT6Code</t>
+  </si>
+  <si>
+    <t>GT7Code</t>
+  </si>
+  <si>
+    <t>GT8Code</t>
+  </si>
+  <si>
+    <t>GT2</t>
+  </si>
+  <si>
+    <t>GT3</t>
+  </si>
+  <si>
+    <t>GT4</t>
+  </si>
+  <si>
+    <t>GT5</t>
+  </si>
+  <si>
+    <t>GT6</t>
+  </si>
+  <si>
+    <t>GT7</t>
+  </si>
+  <si>
+    <t>GT8</t>
+  </si>
+  <si>
+    <t>[DP]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GYSId</t>
+  </si>
+  <si>
+    <t>DP1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DP2</t>
+  </si>
+  <si>
+    <t>DP3</t>
+  </si>
+  <si>
+    <t>DP4</t>
+  </si>
+  <si>
+    <t>DP5</t>
+  </si>
+  <si>
+    <t>DP6</t>
+  </si>
+  <si>
+    <t>DP7</t>
+  </si>
+  <si>
+    <t>DP8</t>
+  </si>
+  <si>
+    <t>[DW]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GTId</t>
+  </si>
+  <si>
+    <t>DPId</t>
+  </si>
+  <si>
+    <t>DW1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DW2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DW3</t>
+  </si>
+  <si>
+    <t>DW4</t>
+  </si>
+  <si>
+    <t>DW5</t>
+  </si>
+  <si>
+    <t>DW6</t>
+  </si>
+  <si>
+    <t>DW7</t>
+  </si>
+  <si>
+    <t>DW8</t>
+  </si>
+  <si>
+    <t>DW9</t>
+  </si>
+  <si>
+    <t>DW10</t>
+  </si>
+  <si>
+    <t>[FG]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FG1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FG2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FG1Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FG2Note</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FG3</t>
+  </si>
+  <si>
+    <t>FG4</t>
+  </si>
+  <si>
+    <t>FG3Note</t>
+  </si>
+  <si>
+    <t>FG4Note</t>
+  </si>
+  <si>
+    <t>FG5</t>
+  </si>
+  <si>
+    <t>FG5Note</t>
+  </si>
+  <si>
+    <t>FG6</t>
+  </si>
+  <si>
+    <t>FG6Note</t>
+  </si>
+  <si>
+    <t>[Tester]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tester1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tester2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tester3</t>
+  </si>
+  <si>
+    <t>Tester4</t>
+  </si>
+  <si>
+    <t>Tester5</t>
+  </si>
+  <si>
+    <t>Tester6</t>
+  </si>
+  <si>
+    <t>[FGTester]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FGId</t>
+  </si>
+  <si>
+    <t>TesterId</t>
+  </si>
+  <si>
+    <t>[WL]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>WL1_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL1_1Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL1_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL1_2Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL1_3</t>
+  </si>
+  <si>
+    <t>WL1_3Code</t>
+  </si>
+  <si>
+    <t>WL1_4</t>
+  </si>
+  <si>
+    <t>WL1_4Code</t>
+  </si>
+  <si>
+    <t>WL1_5</t>
+  </si>
+  <si>
+    <t>WL1_5Code</t>
+  </si>
+  <si>
+    <t>WL1_6</t>
+  </si>
+  <si>
+    <t>WL1_6Code</t>
+  </si>
+  <si>
+    <t>WL2_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL2_1Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL2_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL2_2Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL2_3</t>
+  </si>
+  <si>
+    <t>WL2_3Code</t>
+  </si>
+  <si>
+    <t>WL2_4</t>
+  </si>
+  <si>
+    <t>WL2_4Code</t>
+  </si>
+  <si>
+    <t>WL2_5</t>
+  </si>
+  <si>
+    <t>WL2_5Code</t>
+  </si>
+  <si>
+    <t>WL2_6</t>
+  </si>
+  <si>
+    <t>WL2_6Code</t>
+  </si>
+  <si>
+    <t>WL3_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL3_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL3_3</t>
+  </si>
+  <si>
+    <t>WL3_4</t>
+  </si>
+  <si>
+    <t>WL3_5</t>
+  </si>
+  <si>
+    <t>WL3_6</t>
+  </si>
+  <si>
+    <t>WL3_1Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL3_2Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL3_3Code</t>
+  </si>
+  <si>
+    <t>WL3_4Code</t>
+  </si>
+  <si>
+    <t>WL3_5Code</t>
+  </si>
+  <si>
+    <t>WL3_6Code</t>
+  </si>
+  <si>
+    <t>[EJZH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WLId</t>
+  </si>
+  <si>
+    <t>WL4_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL4_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL4_3</t>
+  </si>
+  <si>
+    <t>WL4_4</t>
+  </si>
+  <si>
+    <t>WL4_5</t>
+  </si>
+  <si>
+    <t>WL4_6</t>
+  </si>
+  <si>
+    <t>WL5_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL5_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL5_3</t>
+  </si>
+  <si>
+    <t>WL5_4</t>
+  </si>
+  <si>
+    <t>WL5_5</t>
+  </si>
+  <si>
+    <t>WL5_6</t>
+  </si>
+  <si>
+    <t>WL6_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL6_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL6_3</t>
+  </si>
+  <si>
+    <t>WL6_4</t>
+  </si>
+  <si>
+    <t>WL6_5</t>
+  </si>
+  <si>
+    <t>WL6_6</t>
+  </si>
+  <si>
+    <t>WL4_1Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL4_2Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL4_3Code</t>
+  </si>
+  <si>
+    <t>WL4_4Code</t>
+  </si>
+  <si>
+    <t>WL4_5Code</t>
+  </si>
+  <si>
+    <t>WL4_6Code</t>
+  </si>
+  <si>
+    <t>WL5_1Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL5_2Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL5_3Code</t>
+  </si>
+  <si>
+    <t>WL5_4Code</t>
+  </si>
+  <si>
+    <t>WL5_5Code</t>
+  </si>
+  <si>
+    <t>WL5_6Code</t>
+  </si>
+  <si>
+    <t>WL6_1Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL6_2Code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>WL6_3Code</t>
+  </si>
+  <si>
+    <t>WL6_4Code</t>
+  </si>
+  <si>
+    <t>WL6_5Code</t>
+  </si>
+  <si>
+    <t>WL6_6Code</t>
+  </si>
+  <si>
+    <t>EJZH1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EJZH2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EJZH3</t>
+  </si>
+  <si>
+    <t>EJZH4</t>
+  </si>
+  <si>
+    <t>EJZH5</t>
+  </si>
+  <si>
+    <t>EJZH6</t>
+  </si>
+  <si>
+    <t>EJZHId</t>
+  </si>
+  <si>
+    <t>FGTesterId</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>[EJZH_FGTester]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[EJZH_SJWL]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[YJZH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YJZH1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YJZH2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YJZH3</t>
+  </si>
+  <si>
+    <t>YJZH4</t>
+  </si>
+  <si>
+    <t>YJZHId</t>
+  </si>
+  <si>
+    <t>[GT_YJZH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT_YJZH1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT_YJZH2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GT_YJZH3</t>
+  </si>
+  <si>
+    <t>GT_YJZH4</t>
+  </si>
+  <si>
+    <t>GT_YJZH5</t>
+  </si>
+  <si>
+    <t>GT_YJZH6</t>
+  </si>
+  <si>
+    <t>GT_YJZH7</t>
+  </si>
+  <si>
+    <t>GT_YJZH8</t>
+  </si>
+  <si>
+    <t>GT_YJZH9</t>
+  </si>
+  <si>
+    <t>[YJZH_EJZH]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YJZH_XGT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YJZH_XGT2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YJZH_XGT3</t>
+  </si>
+  <si>
+    <t>YJZH_XGT4</t>
+  </si>
+  <si>
+    <t>YJZH_XGT5</t>
+  </si>
+  <si>
+    <t>YJZH_XGT6</t>
+  </si>
+  <si>
+    <t>YJZH_XGT7</t>
+  </si>
+  <si>
+    <t>YJZH_XGT8</t>
+  </si>
+  <si>
+    <t>EJZH_XGT1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EJZH_XGT2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EJZH_XGT3</t>
+  </si>
+  <si>
+    <t>EJZH_XGT4</t>
+  </si>
+  <si>
+    <t>EJZH_XGT5</t>
+  </si>
+  <si>
+    <t>EJZH_XGT6</t>
+  </si>
+  <si>
+    <t>EJZH_XGT7</t>
+  </si>
+  <si>
+    <t>EJZH_XGT8</t>
+  </si>
+  <si>
+    <t>[YJZHXGT]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[EJZHXGT]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EJZHId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -368,7 +1046,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -402,6 +1080,11 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -420,7 +1103,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -480,11 +1163,104 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="151">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -514,6 +1290,52 @@
     <cellStyle name="超链接" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -543,6 +1365,52 @@
     <cellStyle name="访问过的超链接" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -872,10 +1740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D144"/>
+  <dimension ref="A1:H343"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A309" workbookViewId="0">
+      <selection activeCell="C333" sqref="C333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -991,7 +1859,7 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" t="b">
         <v>1</v>
@@ -1005,7 +1873,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C14" t="b">
         <v>1</v>
@@ -1019,7 +1887,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1067,7 +1935,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1075,7 +1943,7 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1083,7 +1951,7 @@
         <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1091,7 +1959,7 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1252,7 +2120,7 @@
         <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D39" t="s">
         <v>24</v>
@@ -1266,7 +2134,7 @@
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
         <v>24</v>
@@ -1280,7 +2148,7 @@
         <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D41" t="s">
         <v>24</v>
@@ -1294,7 +2162,7 @@
         <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
         <v>24</v>
@@ -1308,7 +2176,7 @@
         <v>36</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>103</v>
       </c>
       <c r="D43" t="s">
         <v>24</v>
@@ -1322,7 +2190,7 @@
         <v>36</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
         <v>24</v>
@@ -1336,7 +2204,7 @@
         <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
       <c r="D45" t="s">
         <v>24</v>
@@ -1350,7 +2218,7 @@
         <v>36</v>
       </c>
       <c r="C46" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="D46" t="s">
         <v>24</v>
@@ -1364,7 +2232,7 @@
         <v>36</v>
       </c>
       <c r="C47" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="D47" t="s">
         <v>24</v>
@@ -1378,7 +2246,7 @@
         <v>36</v>
       </c>
       <c r="C48" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="D48" t="s">
         <v>24</v>
@@ -1392,7 +2260,7 @@
         <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="D49" t="s">
         <v>24</v>
@@ -1406,7 +2274,7 @@
         <v>36</v>
       </c>
       <c r="C50" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="D50" t="s">
         <v>24</v>
@@ -1417,10 +2285,10 @@
         <v>22</v>
       </c>
       <c r="B51" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C51" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D51" t="s">
         <v>24</v>
@@ -1431,10 +2299,10 @@
         <v>23</v>
       </c>
       <c r="B52" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" t="s">
         <v>39</v>
-      </c>
-      <c r="C52" t="s">
-        <v>41</v>
       </c>
       <c r="D52" t="s">
         <v>24</v>
@@ -1445,10 +2313,10 @@
         <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D53" t="s">
         <v>24</v>
@@ -1459,10 +2327,10 @@
         <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D54" t="s">
         <v>24</v>
@@ -1473,10 +2341,10 @@
         <v>26</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C55" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
         <v>24</v>
@@ -1487,10 +2355,10 @@
         <v>27</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D56" t="s">
         <v>24</v>
@@ -1501,10 +2369,10 @@
         <v>28</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C57" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D57" t="s">
         <v>24</v>
@@ -1515,10 +2383,10 @@
         <v>29</v>
       </c>
       <c r="B58" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C58" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D58" t="s">
         <v>24</v>
@@ -1529,10 +2397,10 @@
         <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D59" t="s">
         <v>24</v>
@@ -1543,10 +2411,10 @@
         <v>31</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="D60" t="s">
         <v>24</v>
@@ -1557,10 +2425,10 @@
         <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D61" t="s">
         <v>24</v>
@@ -1571,10 +2439,10 @@
         <v>33</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C62" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="D62" t="s">
         <v>24</v>
@@ -1585,10 +2453,10 @@
         <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C63" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D63" t="s">
         <v>24</v>
@@ -1599,10 +2467,10 @@
         <v>35</v>
       </c>
       <c r="B64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C64" t="s">
         <v>42</v>
-      </c>
-      <c r="C64" t="s">
-        <v>44</v>
       </c>
       <c r="D64" t="s">
         <v>24</v>
@@ -1613,10 +2481,10 @@
         <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C65" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D65" t="s">
         <v>24</v>
@@ -1627,10 +2495,10 @@
         <v>37</v>
       </c>
       <c r="B66" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C66" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D66" t="s">
         <v>24</v>
@@ -1641,10 +2509,10 @@
         <v>38</v>
       </c>
       <c r="B67" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C67" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D67" t="s">
         <v>24</v>
@@ -1655,10 +2523,10 @@
         <v>39</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D68" t="s">
         <v>24</v>
@@ -1669,10 +2537,10 @@
         <v>40</v>
       </c>
       <c r="B69" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C69" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D69" t="s">
         <v>24</v>
@@ -1683,10 +2551,10 @@
         <v>41</v>
       </c>
       <c r="B70" t="s">
+        <v>43</v>
+      </c>
+      <c r="C70" t="s">
         <v>45</v>
-      </c>
-      <c r="C70" t="s">
-        <v>47</v>
       </c>
       <c r="D70" t="s">
         <v>24</v>
@@ -1697,10 +2565,10 @@
         <v>42</v>
       </c>
       <c r="B71" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C71" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D71" t="s">
         <v>24</v>
@@ -1711,10 +2579,10 @@
         <v>43</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C72" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D72" t="s">
         <v>24</v>
@@ -1725,10 +2593,10 @@
         <v>44</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C73" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D73" t="s">
         <v>24</v>
@@ -1739,10 +2607,10 @@
         <v>45</v>
       </c>
       <c r="B74" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C74" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D74" t="s">
         <v>24</v>
@@ -1750,15 +2618,15 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B77" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -1779,15 +2647,15 @@
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1808,15 +2676,15 @@
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B87" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1869,15 +2737,15 @@
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B96" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1930,15 +2798,15 @@
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B105" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2007,15 +2875,15 @@
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B116" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2084,15 +2952,15 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B127" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2145,15 +3013,15 @@
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B136" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2206,7 +3074,2557 @@
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>94</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="A145" t="s">
+        <v>118</v>
+      </c>
+      <c r="B145" t="s">
+        <v>119</v>
+      </c>
+      <c r="C145" t="s">
+        <v>111</v>
+      </c>
+      <c r="D145" t="s">
+        <v>48</v>
+      </c>
+      <c r="E145" t="s">
+        <v>112</v>
+      </c>
+      <c r="F145" t="s">
+        <v>113</v>
+      </c>
+      <c r="G145" t="s">
+        <v>114</v>
+      </c>
+      <c r="H145" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146" t="s">
+        <v>100</v>
+      </c>
+      <c r="C146" t="s">
+        <v>101</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
+        <v>102</v>
+      </c>
+      <c r="F146">
+        <v>14</v>
+      </c>
+      <c r="G146">
+        <v>6</v>
+      </c>
+      <c r="H146" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147">
+        <v>2</v>
+      </c>
+      <c r="B147" t="s">
+        <v>132</v>
+      </c>
+      <c r="C147" t="s">
+        <v>125</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+      <c r="E147" t="s">
+        <v>102</v>
+      </c>
+      <c r="F147">
+        <v>15</v>
+      </c>
+      <c r="G147">
+        <v>6</v>
+      </c>
+      <c r="H147" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148">
+        <v>3</v>
+      </c>
+      <c r="B148" t="s">
+        <v>133</v>
+      </c>
+      <c r="C148" t="s">
+        <v>126</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148" t="s">
+        <v>123</v>
+      </c>
+      <c r="F148">
+        <v>16</v>
+      </c>
+      <c r="G148">
+        <v>7</v>
+      </c>
+      <c r="H148" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149">
+        <v>4</v>
+      </c>
+      <c r="B149" t="s">
+        <v>134</v>
+      </c>
+      <c r="C149" t="s">
+        <v>127</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149" t="s">
+        <v>123</v>
+      </c>
+      <c r="F149">
+        <v>17</v>
+      </c>
+      <c r="G149">
+        <v>7</v>
+      </c>
+      <c r="H149" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="A150">
+        <v>5</v>
+      </c>
+      <c r="B150" t="s">
+        <v>135</v>
+      </c>
+      <c r="C150" t="s">
+        <v>128</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+      <c r="E150" t="s">
+        <v>124</v>
+      </c>
+      <c r="F150">
+        <v>18</v>
+      </c>
+      <c r="G150">
+        <v>8</v>
+      </c>
+      <c r="H150" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="A151">
+        <v>6</v>
+      </c>
+      <c r="B151" t="s">
+        <v>136</v>
+      </c>
+      <c r="C151" t="s">
+        <v>129</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151" t="s">
+        <v>124</v>
+      </c>
+      <c r="F151">
+        <v>19</v>
+      </c>
+      <c r="G151">
+        <v>8</v>
+      </c>
+      <c r="H151" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="A152">
+        <v>7</v>
+      </c>
+      <c r="B152" t="s">
+        <v>137</v>
+      </c>
+      <c r="C152" t="s">
+        <v>130</v>
+      </c>
+      <c r="D152">
+        <v>2</v>
+      </c>
+      <c r="E152" t="s">
+        <v>102</v>
+      </c>
+      <c r="F152">
+        <v>20</v>
+      </c>
+      <c r="G152">
+        <v>12</v>
+      </c>
+      <c r="H152" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="A153">
+        <v>8</v>
+      </c>
+      <c r="B153" t="s">
+        <v>138</v>
+      </c>
+      <c r="C153" t="s">
+        <v>131</v>
+      </c>
+      <c r="D153">
+        <v>2</v>
+      </c>
+      <c r="E153" t="s">
+        <v>102</v>
+      </c>
+      <c r="F153">
+        <v>21</v>
+      </c>
+      <c r="G153">
+        <v>13</v>
+      </c>
+      <c r="H153" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="A155" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="A156" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157" t="s">
+        <v>141</v>
+      </c>
+      <c r="C157">
+        <v>1</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="A158">
+        <v>2</v>
+      </c>
+      <c r="B158" t="s">
+        <v>142</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="A159">
+        <v>3</v>
+      </c>
+      <c r="B159" t="s">
+        <v>143</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="A160">
+        <v>4</v>
+      </c>
+      <c r="B160" t="s">
+        <v>144</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+      <c r="D160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161">
+        <v>5</v>
+      </c>
+      <c r="B161" t="s">
+        <v>145</v>
+      </c>
+      <c r="C161">
+        <v>2</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="A162">
+        <v>6</v>
+      </c>
+      <c r="B162" t="s">
+        <v>146</v>
+      </c>
+      <c r="C162">
+        <v>2</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163">
+        <v>7</v>
+      </c>
+      <c r="B163" t="s">
+        <v>147</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+      <c r="D163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164">
+        <v>8</v>
+      </c>
+      <c r="B164" t="s">
+        <v>148</v>
+      </c>
+      <c r="C164">
+        <v>2</v>
+      </c>
+      <c r="D164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168">
+        <v>1</v>
+      </c>
+      <c r="B168" t="s">
+        <v>152</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+      <c r="D168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169">
+        <v>2</v>
+      </c>
+      <c r="B169" t="s">
+        <v>153</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170">
+        <v>3</v>
+      </c>
+      <c r="B170" t="s">
+        <v>154</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171">
+        <v>4</v>
+      </c>
+      <c r="B171" t="s">
+        <v>155</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+      <c r="D171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172">
+        <v>5</v>
+      </c>
+      <c r="B172" t="s">
+        <v>156</v>
+      </c>
+      <c r="C172">
+        <v>2</v>
+      </c>
+      <c r="D172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173">
+        <v>6</v>
+      </c>
+      <c r="B173" t="s">
+        <v>157</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+      <c r="D173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174">
+        <v>7</v>
+      </c>
+      <c r="B174" t="s">
+        <v>158</v>
+      </c>
+      <c r="C174">
+        <v>7</v>
+      </c>
+      <c r="D174">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175">
+        <v>8</v>
+      </c>
+      <c r="B175" t="s">
+        <v>159</v>
+      </c>
+      <c r="C175">
+        <v>7</v>
+      </c>
+      <c r="D175">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176">
+        <v>9</v>
+      </c>
+      <c r="B176" t="s">
+        <v>160</v>
+      </c>
+      <c r="C176">
+        <v>8</v>
+      </c>
+      <c r="D176">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177">
+        <v>10</v>
+      </c>
+      <c r="B177" t="s">
+        <v>161</v>
+      </c>
+      <c r="C177">
+        <v>8</v>
+      </c>
+      <c r="D177">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181">
+        <v>1</v>
+      </c>
+      <c r="B181" t="s">
+        <v>163</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+      <c r="D181" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182">
+        <v>2</v>
+      </c>
+      <c r="B182" t="s">
+        <v>164</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+      <c r="D182" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183">
+        <v>3</v>
+      </c>
+      <c r="B183" t="s">
+        <v>167</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184">
+        <v>4</v>
+      </c>
+      <c r="B184" t="s">
+        <v>168</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+      <c r="D184" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185">
+        <v>5</v>
+      </c>
+      <c r="B185" t="s">
+        <v>171</v>
+      </c>
+      <c r="C185">
+        <v>2</v>
+      </c>
+      <c r="D185" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186">
+        <v>6</v>
+      </c>
+      <c r="B186" t="s">
+        <v>173</v>
+      </c>
+      <c r="C186">
+        <v>2</v>
+      </c>
+      <c r="D186" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190">
+        <v>1</v>
+      </c>
+      <c r="B190" t="s">
+        <v>176</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191">
+        <v>2</v>
+      </c>
+      <c r="B191" t="s">
+        <v>177</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192">
+        <v>3</v>
+      </c>
+      <c r="B192" t="s">
+        <v>178</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193">
+        <v>4</v>
+      </c>
+      <c r="B193" t="s">
+        <v>179</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194">
+        <v>5</v>
+      </c>
+      <c r="B194" t="s">
+        <v>180</v>
+      </c>
+      <c r="C194">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195">
+        <v>6</v>
+      </c>
+      <c r="B195" t="s">
+        <v>181</v>
+      </c>
+      <c r="C195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199">
+        <v>1</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200">
+        <v>2</v>
+      </c>
+      <c r="B200">
+        <v>1</v>
+      </c>
+      <c r="C200">
+        <v>2</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201">
+        <v>3</v>
+      </c>
+      <c r="B201">
+        <v>1</v>
+      </c>
+      <c r="C201">
+        <v>3</v>
+      </c>
+      <c r="D201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202">
+        <v>4</v>
+      </c>
+      <c r="B202">
+        <v>1</v>
+      </c>
+      <c r="C202">
+        <v>4</v>
+      </c>
+      <c r="D202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203">
+        <v>5</v>
+      </c>
+      <c r="B203">
+        <v>2</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204">
+        <v>6</v>
+      </c>
+      <c r="B204">
+        <v>2</v>
+      </c>
+      <c r="C204">
+        <v>2</v>
+      </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205">
+        <v>7</v>
+      </c>
+      <c r="B205">
+        <v>5</v>
+      </c>
+      <c r="C205">
+        <v>5</v>
+      </c>
+      <c r="D205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206">
+        <v>8</v>
+      </c>
+      <c r="B206">
+        <v>5</v>
+      </c>
+      <c r="C206">
+        <v>6</v>
+      </c>
+      <c r="D206">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207">
+        <v>9</v>
+      </c>
+      <c r="B207">
+        <v>6</v>
+      </c>
+      <c r="C207">
+        <v>5</v>
+      </c>
+      <c r="D207">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208">
+        <v>10</v>
+      </c>
+      <c r="B208">
+        <v>6</v>
+      </c>
+      <c r="C208">
+        <v>6</v>
+      </c>
+      <c r="D208">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7">
+      <c r="A210" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7">
+      <c r="A211" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="E211" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G211" s="1"/>
+    </row>
+    <row r="212" spans="1:7">
+      <c r="A212">
+        <v>1</v>
+      </c>
+      <c r="B212" t="s">
+        <v>187</v>
+      </c>
+      <c r="C212" t="s">
+        <v>188</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+      <c r="E212">
+        <v>1</v>
+      </c>
+      <c r="F212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7">
+      <c r="A213">
+        <v>2</v>
+      </c>
+      <c r="B213" t="s">
+        <v>189</v>
+      </c>
+      <c r="C213" t="s">
+        <v>190</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+      <c r="E213">
+        <v>1</v>
+      </c>
+      <c r="F213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7">
+      <c r="A214">
+        <v>3</v>
+      </c>
+      <c r="B214" t="s">
+        <v>191</v>
+      </c>
+      <c r="C214" t="s">
+        <v>192</v>
+      </c>
+      <c r="D214">
+        <v>1</v>
+      </c>
+      <c r="E214">
+        <v>1</v>
+      </c>
+      <c r="F214">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7">
+      <c r="A215">
+        <v>4</v>
+      </c>
+      <c r="B215" t="s">
+        <v>193</v>
+      </c>
+      <c r="C215" t="s">
+        <v>194</v>
+      </c>
+      <c r="D215">
+        <v>1</v>
+      </c>
+      <c r="E215">
+        <v>1</v>
+      </c>
+      <c r="F215">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7">
+      <c r="A216">
+        <v>5</v>
+      </c>
+      <c r="B216" t="s">
+        <v>195</v>
+      </c>
+      <c r="C216" t="s">
+        <v>196</v>
+      </c>
+      <c r="D216">
+        <v>1</v>
+      </c>
+      <c r="E216">
+        <v>1</v>
+      </c>
+      <c r="F216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7">
+      <c r="A217">
+        <v>6</v>
+      </c>
+      <c r="B217" t="s">
+        <v>197</v>
+      </c>
+      <c r="C217" t="s">
+        <v>198</v>
+      </c>
+      <c r="D217">
+        <v>1</v>
+      </c>
+      <c r="E217">
+        <v>1</v>
+      </c>
+      <c r="F217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7">
+      <c r="A218">
+        <v>7</v>
+      </c>
+      <c r="B218" t="s">
+        <v>199</v>
+      </c>
+      <c r="C218" t="s">
+        <v>200</v>
+      </c>
+      <c r="D218">
+        <v>2</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+      <c r="F218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7">
+      <c r="A219">
+        <v>8</v>
+      </c>
+      <c r="B219" t="s">
+        <v>201</v>
+      </c>
+      <c r="C219" t="s">
+        <v>202</v>
+      </c>
+      <c r="D219">
+        <v>2</v>
+      </c>
+      <c r="E219">
+        <v>1</v>
+      </c>
+      <c r="F219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7">
+      <c r="A220">
+        <v>9</v>
+      </c>
+      <c r="B220" t="s">
+        <v>203</v>
+      </c>
+      <c r="C220" t="s">
+        <v>204</v>
+      </c>
+      <c r="D220">
+        <v>2</v>
+      </c>
+      <c r="E220">
+        <v>1</v>
+      </c>
+      <c r="F220">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7">
+      <c r="A221">
+        <v>10</v>
+      </c>
+      <c r="B221" t="s">
+        <v>205</v>
+      </c>
+      <c r="C221" t="s">
+        <v>206</v>
+      </c>
+      <c r="D221">
+        <v>2</v>
+      </c>
+      <c r="E221">
+        <v>1</v>
+      </c>
+      <c r="F221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7">
+      <c r="A222">
+        <v>11</v>
+      </c>
+      <c r="B222" t="s">
+        <v>207</v>
+      </c>
+      <c r="C222" t="s">
+        <v>208</v>
+      </c>
+      <c r="D222">
+        <v>2</v>
+      </c>
+      <c r="E222">
+        <v>1</v>
+      </c>
+      <c r="F222">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7">
+      <c r="A223">
+        <v>12</v>
+      </c>
+      <c r="B223" t="s">
+        <v>209</v>
+      </c>
+      <c r="C223" t="s">
+        <v>210</v>
+      </c>
+      <c r="D223">
+        <v>2</v>
+      </c>
+      <c r="E223">
+        <v>1</v>
+      </c>
+      <c r="F223">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7">
+      <c r="A224">
+        <v>13</v>
+      </c>
+      <c r="B224" t="s">
+        <v>211</v>
+      </c>
+      <c r="C224" t="s">
+        <v>217</v>
+      </c>
+      <c r="D224">
+        <v>3</v>
+      </c>
+      <c r="E224">
+        <v>1</v>
+      </c>
+      <c r="F224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6">
+      <c r="A225">
+        <v>14</v>
+      </c>
+      <c r="B225" t="s">
+        <v>212</v>
+      </c>
+      <c r="C225" t="s">
+        <v>218</v>
+      </c>
+      <c r="D225">
+        <v>3</v>
+      </c>
+      <c r="E225">
+        <v>1</v>
+      </c>
+      <c r="F225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6">
+      <c r="A226">
+        <v>15</v>
+      </c>
+      <c r="B226" t="s">
+        <v>213</v>
+      </c>
+      <c r="C226" t="s">
+        <v>219</v>
+      </c>
+      <c r="D226">
+        <v>3</v>
+      </c>
+      <c r="E226">
+        <v>1</v>
+      </c>
+      <c r="F226">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6">
+      <c r="A227">
+        <v>16</v>
+      </c>
+      <c r="B227" t="s">
+        <v>214</v>
+      </c>
+      <c r="C227" t="s">
+        <v>220</v>
+      </c>
+      <c r="D227">
+        <v>3</v>
+      </c>
+      <c r="E227">
+        <v>1</v>
+      </c>
+      <c r="F227">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6">
+      <c r="A228">
+        <v>17</v>
+      </c>
+      <c r="B228" t="s">
+        <v>215</v>
+      </c>
+      <c r="C228" t="s">
+        <v>221</v>
+      </c>
+      <c r="D228">
+        <v>3</v>
+      </c>
+      <c r="E228">
+        <v>1</v>
+      </c>
+      <c r="F228">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6">
+      <c r="A229">
+        <v>18</v>
+      </c>
+      <c r="B229" t="s">
+        <v>216</v>
+      </c>
+      <c r="C229" t="s">
+        <v>222</v>
+      </c>
+      <c r="D229">
+        <v>3</v>
+      </c>
+      <c r="E229">
+        <v>1</v>
+      </c>
+      <c r="F229">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6">
+      <c r="A230">
+        <v>19</v>
+      </c>
+      <c r="B230" t="s">
+        <v>225</v>
+      </c>
+      <c r="C230" t="s">
+        <v>243</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+      <c r="E230">
+        <v>2</v>
+      </c>
+      <c r="F230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6">
+      <c r="A231">
+        <v>20</v>
+      </c>
+      <c r="B231" t="s">
+        <v>226</v>
+      </c>
+      <c r="C231" t="s">
+        <v>244</v>
+      </c>
+      <c r="D231">
+        <v>1</v>
+      </c>
+      <c r="E231">
+        <v>2</v>
+      </c>
+      <c r="F231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6">
+      <c r="A232">
+        <v>21</v>
+      </c>
+      <c r="B232" t="s">
+        <v>227</v>
+      </c>
+      <c r="C232" t="s">
+        <v>245</v>
+      </c>
+      <c r="D232">
+        <v>1</v>
+      </c>
+      <c r="E232">
+        <v>2</v>
+      </c>
+      <c r="F232">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6">
+      <c r="A233">
+        <v>22</v>
+      </c>
+      <c r="B233" t="s">
+        <v>228</v>
+      </c>
+      <c r="C233" t="s">
+        <v>246</v>
+      </c>
+      <c r="D233">
+        <v>1</v>
+      </c>
+      <c r="E233">
+        <v>2</v>
+      </c>
+      <c r="F233">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6">
+      <c r="A234">
+        <v>23</v>
+      </c>
+      <c r="B234" t="s">
+        <v>229</v>
+      </c>
+      <c r="C234" t="s">
+        <v>247</v>
+      </c>
+      <c r="D234">
+        <v>1</v>
+      </c>
+      <c r="E234">
+        <v>2</v>
+      </c>
+      <c r="F234">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6">
+      <c r="A235">
+        <v>24</v>
+      </c>
+      <c r="B235" t="s">
+        <v>230</v>
+      </c>
+      <c r="C235" t="s">
+        <v>248</v>
+      </c>
+      <c r="D235">
+        <v>1</v>
+      </c>
+      <c r="E235">
+        <v>2</v>
+      </c>
+      <c r="F235">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6">
+      <c r="A236">
+        <v>25</v>
+      </c>
+      <c r="B236" t="s">
+        <v>231</v>
+      </c>
+      <c r="C236" t="s">
+        <v>249</v>
+      </c>
+      <c r="D236">
+        <v>2</v>
+      </c>
+      <c r="E236">
+        <v>2</v>
+      </c>
+      <c r="F236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6">
+      <c r="A237">
+        <v>26</v>
+      </c>
+      <c r="B237" t="s">
+        <v>232</v>
+      </c>
+      <c r="C237" t="s">
+        <v>250</v>
+      </c>
+      <c r="D237">
+        <v>2</v>
+      </c>
+      <c r="E237">
+        <v>2</v>
+      </c>
+      <c r="F237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6">
+      <c r="A238">
+        <v>27</v>
+      </c>
+      <c r="B238" t="s">
+        <v>233</v>
+      </c>
+      <c r="C238" t="s">
+        <v>251</v>
+      </c>
+      <c r="D238">
+        <v>2</v>
+      </c>
+      <c r="E238">
+        <v>2</v>
+      </c>
+      <c r="F238">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6">
+      <c r="A239">
+        <v>28</v>
+      </c>
+      <c r="B239" t="s">
+        <v>234</v>
+      </c>
+      <c r="C239" t="s">
+        <v>252</v>
+      </c>
+      <c r="D239">
+        <v>2</v>
+      </c>
+      <c r="E239">
+        <v>2</v>
+      </c>
+      <c r="F239">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6">
+      <c r="A240">
+        <v>29</v>
+      </c>
+      <c r="B240" t="s">
+        <v>235</v>
+      </c>
+      <c r="C240" t="s">
+        <v>253</v>
+      </c>
+      <c r="D240">
+        <v>2</v>
+      </c>
+      <c r="E240">
+        <v>2</v>
+      </c>
+      <c r="F240">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6">
+      <c r="A241">
+        <v>30</v>
+      </c>
+      <c r="B241" t="s">
+        <v>236</v>
+      </c>
+      <c r="C241" t="s">
+        <v>254</v>
+      </c>
+      <c r="D241">
+        <v>2</v>
+      </c>
+      <c r="E241">
+        <v>2</v>
+      </c>
+      <c r="F241">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6">
+      <c r="A242">
+        <v>31</v>
+      </c>
+      <c r="B242" t="s">
+        <v>237</v>
+      </c>
+      <c r="C242" t="s">
+        <v>255</v>
+      </c>
+      <c r="D242">
+        <v>3</v>
+      </c>
+      <c r="E242">
+        <v>2</v>
+      </c>
+      <c r="F242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6">
+      <c r="A243">
+        <v>32</v>
+      </c>
+      <c r="B243" t="s">
+        <v>238</v>
+      </c>
+      <c r="C243" t="s">
+        <v>256</v>
+      </c>
+      <c r="D243">
+        <v>3</v>
+      </c>
+      <c r="E243">
+        <v>2</v>
+      </c>
+      <c r="F243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6">
+      <c r="A244">
+        <v>33</v>
+      </c>
+      <c r="B244" t="s">
+        <v>239</v>
+      </c>
+      <c r="C244" t="s">
+        <v>257</v>
+      </c>
+      <c r="D244">
+        <v>3</v>
+      </c>
+      <c r="E244">
+        <v>2</v>
+      </c>
+      <c r="F244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6">
+      <c r="A245">
+        <v>34</v>
+      </c>
+      <c r="B245" t="s">
+        <v>240</v>
+      </c>
+      <c r="C245" t="s">
+        <v>258</v>
+      </c>
+      <c r="D245">
+        <v>3</v>
+      </c>
+      <c r="E245">
+        <v>2</v>
+      </c>
+      <c r="F245">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6">
+      <c r="A246">
+        <v>35</v>
+      </c>
+      <c r="B246" t="s">
+        <v>241</v>
+      </c>
+      <c r="C246" t="s">
+        <v>259</v>
+      </c>
+      <c r="D246">
+        <v>3</v>
+      </c>
+      <c r="E246">
+        <v>2</v>
+      </c>
+      <c r="F246">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6">
+      <c r="A247">
+        <v>36</v>
+      </c>
+      <c r="B247" t="s">
+        <v>242</v>
+      </c>
+      <c r="C247" t="s">
+        <v>260</v>
+      </c>
+      <c r="D247">
+        <v>3</v>
+      </c>
+      <c r="E247">
+        <v>2</v>
+      </c>
+      <c r="F247">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6">
+      <c r="A252" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6">
+      <c r="A253" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6">
+      <c r="A254">
+        <v>1</v>
+      </c>
+      <c r="B254" t="s">
+        <v>261</v>
+      </c>
+      <c r="C254">
+        <v>7</v>
+      </c>
+      <c r="D254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6">
+      <c r="A255">
+        <v>2</v>
+      </c>
+      <c r="B255" t="s">
+        <v>262</v>
+      </c>
+      <c r="C255">
+        <v>8</v>
+      </c>
+      <c r="D255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6">
+      <c r="A256">
+        <v>3</v>
+      </c>
+      <c r="B256" t="s">
+        <v>263</v>
+      </c>
+      <c r="C256">
+        <v>9</v>
+      </c>
+      <c r="D256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
+      <c r="A257">
+        <v>4</v>
+      </c>
+      <c r="B257" t="s">
+        <v>264</v>
+      </c>
+      <c r="C257">
+        <v>25</v>
+      </c>
+      <c r="D257">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
+      <c r="A258">
+        <v>5</v>
+      </c>
+      <c r="B258" t="s">
+        <v>265</v>
+      </c>
+      <c r="C258">
+        <v>26</v>
+      </c>
+      <c r="D258">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259">
+        <v>6</v>
+      </c>
+      <c r="B259" t="s">
+        <v>266</v>
+      </c>
+      <c r="C259">
+        <v>27</v>
+      </c>
+      <c r="D259">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4">
+      <c r="A262" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4">
+      <c r="A263">
+        <v>1</v>
+      </c>
+      <c r="B263">
+        <v>1</v>
+      </c>
+      <c r="C263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4">
+      <c r="A264">
+        <v>1</v>
+      </c>
+      <c r="B264">
+        <v>2</v>
+      </c>
+      <c r="C264">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4">
+      <c r="A265">
+        <v>1</v>
+      </c>
+      <c r="B265">
+        <v>3</v>
+      </c>
+      <c r="C265">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4">
+      <c r="A266">
+        <v>1</v>
+      </c>
+      <c r="B266">
+        <v>4</v>
+      </c>
+      <c r="C266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4">
+      <c r="A267">
+        <v>1</v>
+      </c>
+      <c r="B267">
+        <v>5</v>
+      </c>
+      <c r="C267">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4">
+      <c r="A268">
+        <v>1</v>
+      </c>
+      <c r="B268">
+        <v>6</v>
+      </c>
+      <c r="C268">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4">
+      <c r="A269">
+        <v>4</v>
+      </c>
+      <c r="B269">
+        <v>7</v>
+      </c>
+      <c r="C269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4">
+      <c r="A270">
+        <v>4</v>
+      </c>
+      <c r="B270">
+        <v>8</v>
+      </c>
+      <c r="C270">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4">
+      <c r="A271">
+        <v>4</v>
+      </c>
+      <c r="B271">
+        <v>9</v>
+      </c>
+      <c r="C271">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4">
+      <c r="A272">
+        <v>4</v>
+      </c>
+      <c r="B272">
+        <v>10</v>
+      </c>
+      <c r="C272">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4">
+      <c r="A274" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4">
+      <c r="A275" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4">
+      <c r="A276">
+        <v>1</v>
+      </c>
+      <c r="B276">
+        <v>13</v>
+      </c>
+      <c r="C276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4">
+      <c r="A277">
+        <v>1</v>
+      </c>
+      <c r="B277">
+        <v>14</v>
+      </c>
+      <c r="C277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4">
+      <c r="A278">
+        <v>1</v>
+      </c>
+      <c r="B278">
+        <v>15</v>
+      </c>
+      <c r="C278">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4">
+      <c r="A279">
+        <v>1</v>
+      </c>
+      <c r="B279">
+        <v>16</v>
+      </c>
+      <c r="C279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4">
+      <c r="A280">
+        <v>1</v>
+      </c>
+      <c r="B280">
+        <v>17</v>
+      </c>
+      <c r="C280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4">
+      <c r="A281">
+        <v>1</v>
+      </c>
+      <c r="B281">
+        <v>18</v>
+      </c>
+      <c r="C281">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
+      <c r="A282">
+        <v>4</v>
+      </c>
+      <c r="B282">
+        <v>31</v>
+      </c>
+      <c r="C282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
+      <c r="A283">
+        <v>4</v>
+      </c>
+      <c r="B283">
+        <v>32</v>
+      </c>
+      <c r="C283">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
+      <c r="A284">
+        <v>4</v>
+      </c>
+      <c r="B284">
+        <v>33</v>
+      </c>
+      <c r="C284">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4">
+      <c r="A285">
+        <v>4</v>
+      </c>
+      <c r="B285">
+        <v>34</v>
+      </c>
+      <c r="C285">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4">
+      <c r="A287" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4">
+      <c r="A288" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D288" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4">
+      <c r="A289">
+        <v>1</v>
+      </c>
+      <c r="B289" t="s">
+        <v>273</v>
+      </c>
+      <c r="C289">
+        <v>1</v>
+      </c>
+      <c r="D289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4">
+      <c r="A290">
+        <v>2</v>
+      </c>
+      <c r="B290" t="s">
+        <v>274</v>
+      </c>
+      <c r="C290">
+        <v>2</v>
+      </c>
+      <c r="D290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4">
+      <c r="A291">
+        <v>3</v>
+      </c>
+      <c r="B291" t="s">
+        <v>275</v>
+      </c>
+      <c r="C291">
+        <v>19</v>
+      </c>
+      <c r="D291">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4">
+      <c r="A292">
+        <v>4</v>
+      </c>
+      <c r="B292" t="s">
+        <v>276</v>
+      </c>
+      <c r="C292">
+        <v>20</v>
+      </c>
+      <c r="D292">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4">
+      <c r="A294" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4">
+      <c r="A295" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4">
+      <c r="A296">
+        <v>1</v>
+      </c>
+      <c r="B296">
+        <v>1</v>
+      </c>
+      <c r="C296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4">
+      <c r="A297">
+        <v>1</v>
+      </c>
+      <c r="B297">
+        <v>2</v>
+      </c>
+      <c r="C297">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4">
+      <c r="A298">
+        <v>1</v>
+      </c>
+      <c r="B298">
+        <v>3</v>
+      </c>
+      <c r="C298">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4">
+      <c r="A299">
+        <v>2</v>
+      </c>
+      <c r="B299">
+        <v>3</v>
+      </c>
+      <c r="C299">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4">
+      <c r="A300">
+        <v>2</v>
+      </c>
+      <c r="B300">
+        <v>2</v>
+      </c>
+      <c r="C300">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4">
+      <c r="A301">
+        <v>2</v>
+      </c>
+      <c r="B301">
+        <v>1</v>
+      </c>
+      <c r="C301">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4">
+      <c r="A302">
+        <v>3</v>
+      </c>
+      <c r="B302">
+        <v>4</v>
+      </c>
+      <c r="C302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4">
+      <c r="A303">
+        <v>3</v>
+      </c>
+      <c r="B303">
+        <v>5</v>
+      </c>
+      <c r="C303">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4">
+      <c r="A304">
+        <v>3</v>
+      </c>
+      <c r="B304">
+        <v>6</v>
+      </c>
+      <c r="C304">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4">
+      <c r="A305">
+        <v>4</v>
+      </c>
+      <c r="B305">
+        <v>6</v>
+      </c>
+      <c r="C305">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4">
+      <c r="A306">
+        <v>4</v>
+      </c>
+      <c r="B306">
+        <v>5</v>
+      </c>
+      <c r="C306">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4">
+      <c r="A307">
+        <v>4</v>
+      </c>
+      <c r="B307">
+        <v>4</v>
+      </c>
+      <c r="C307">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4">
+      <c r="A309" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4">
+      <c r="A310" t="s">
+        <v>118</v>
+      </c>
+      <c r="B310" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D310" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4">
+      <c r="A311">
+        <v>1</v>
+      </c>
+      <c r="B311">
+        <v>1</v>
+      </c>
+      <c r="C311">
+        <v>1</v>
+      </c>
+      <c r="D311" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4">
+      <c r="A312">
+        <v>2</v>
+      </c>
+      <c r="B312">
+        <v>1</v>
+      </c>
+      <c r="C312">
+        <v>1</v>
+      </c>
+      <c r="D312" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4">
+      <c r="A313">
+        <v>3</v>
+      </c>
+      <c r="B313">
+        <v>2</v>
+      </c>
+      <c r="C313">
+        <v>1</v>
+      </c>
+      <c r="D313" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4">
+      <c r="A314">
+        <v>4</v>
+      </c>
+      <c r="B314">
+        <v>3</v>
+      </c>
+      <c r="C314">
+        <v>2</v>
+      </c>
+      <c r="D314" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4">
+      <c r="A315">
+        <v>5</v>
+      </c>
+      <c r="B315">
+        <v>4</v>
+      </c>
+      <c r="C315">
+        <v>1</v>
+      </c>
+      <c r="D315" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4">
+      <c r="A316">
+        <v>6</v>
+      </c>
+      <c r="B316">
+        <v>5</v>
+      </c>
+      <c r="C316">
+        <v>2</v>
+      </c>
+      <c r="D316" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4">
+      <c r="A317">
+        <v>7</v>
+      </c>
+      <c r="B317">
+        <v>6</v>
+      </c>
+      <c r="C317">
+        <v>1</v>
+      </c>
+      <c r="D317" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4">
+      <c r="A318">
+        <v>8</v>
+      </c>
+      <c r="B318">
+        <v>7</v>
+      </c>
+      <c r="C318">
+        <v>3</v>
+      </c>
+      <c r="D318" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4">
+      <c r="A319">
+        <v>9</v>
+      </c>
+      <c r="B319">
+        <v>8</v>
+      </c>
+      <c r="C319">
+        <v>4</v>
+      </c>
+      <c r="D319" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3">
+      <c r="A321" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3">
+      <c r="A322" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B322" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3">
+      <c r="A323">
+        <v>1</v>
+      </c>
+      <c r="B323" t="s">
+        <v>289</v>
+      </c>
+      <c r="C323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3">
+      <c r="A324">
+        <v>2</v>
+      </c>
+      <c r="B324" t="s">
+        <v>290</v>
+      </c>
+      <c r="C324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3">
+      <c r="A325">
+        <v>3</v>
+      </c>
+      <c r="B325" t="s">
+        <v>291</v>
+      </c>
+      <c r="C325">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3">
+      <c r="A326">
+        <v>4</v>
+      </c>
+      <c r="B326" t="s">
+        <v>292</v>
+      </c>
+      <c r="C326">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3">
+      <c r="A327">
+        <v>5</v>
+      </c>
+      <c r="B327" t="s">
+        <v>293</v>
+      </c>
+      <c r="C327">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3">
+      <c r="A328">
+        <v>6</v>
+      </c>
+      <c r="B328" t="s">
+        <v>294</v>
+      </c>
+      <c r="C328">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3">
+      <c r="A329">
+        <v>7</v>
+      </c>
+      <c r="B329" t="s">
+        <v>295</v>
+      </c>
+      <c r="C329">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3">
+      <c r="A330">
+        <v>8</v>
+      </c>
+      <c r="B330" t="s">
+        <v>296</v>
+      </c>
+      <c r="C330">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3">
+      <c r="A332" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3">
+      <c r="A333" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3">
+      <c r="A334">
+        <v>1</v>
+      </c>
+      <c r="B334" t="s">
+        <v>297</v>
+      </c>
+      <c r="C334">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3">
+      <c r="A335">
+        <v>2</v>
+      </c>
+      <c r="B335" t="s">
+        <v>298</v>
+      </c>
+      <c r="C335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3">
+      <c r="A336">
+        <v>3</v>
+      </c>
+      <c r="B336" t="s">
+        <v>299</v>
+      </c>
+      <c r="C336">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3">
+      <c r="A337">
+        <v>4</v>
+      </c>
+      <c r="B337" t="s">
+        <v>300</v>
+      </c>
+      <c r="C337">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="A338">
+        <v>5</v>
+      </c>
+      <c r="B338" t="s">
+        <v>301</v>
+      </c>
+      <c r="C338">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3">
+      <c r="A339">
+        <v>6</v>
+      </c>
+      <c r="B339" t="s">
+        <v>302</v>
+      </c>
+      <c r="C339">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="340" spans="1:3">
+      <c r="A340">
+        <v>7</v>
+      </c>
+      <c r="B340" t="s">
+        <v>303</v>
+      </c>
+      <c r="C340">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="341" spans="1:3">
+      <c r="A341">
+        <v>8</v>
+      </c>
+      <c r="B341" t="s">
+        <v>304</v>
+      </c>
+      <c r="C341">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="343" spans="1:3">
+      <c r="A343" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tmp save before adding foreignKey onUpdate onDelete
</commit_message>
<xml_diff>
--- a/tools/initData.xlsx
+++ b/tools/initData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="24640" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="24640" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -1056,8 +1056,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1231,7 +1233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="171">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1316,6 +1318,7 @@
     <cellStyle name="超链接" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1400,6 +1403,7 @@
     <cellStyle name="访问过的超链接" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1732,7 +1736,7 @@
   <dimension ref="A1:H331"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="A300" sqref="A300:XFD300"/>
+      <selection activeCell="M301" sqref="M301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
tmp save after add db Views
</commit_message>
<xml_diff>
--- a/tools/initData.xlsx
+++ b/tools/initData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="0" windowWidth="24640" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="-33620" yWindow="0" windowWidth="24640" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="296">
   <si>
     <t>// 品牌</t>
   </si>
@@ -993,6 +993,9 @@
   <si>
     <t>number</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YJZH5</t>
   </si>
 </sst>
 </file>
@@ -1056,8 +1059,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="171">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1233,7 +1254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="171">
+  <cellStyles count="189">
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
@@ -1319,6 +1340,15 @@
     <cellStyle name="超链接" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="6" builtinId="9" hidden="1"/>
@@ -1404,6 +1434,15 @@
     <cellStyle name="访问过的超链接" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="访问过的超链接" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1733,10 +1772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H331"/>
+  <dimension ref="A1:H336"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A281" workbookViewId="0">
-      <selection activeCell="M301" sqref="M301"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A250" workbookViewId="0">
+      <selection activeCell="G271" sqref="G271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4648,7 +4687,7 @@
         <v>244</v>
       </c>
       <c r="C244">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D244">
         <v>1</v>
@@ -4920,24 +4959,24 @@
     </row>
     <row r="271" spans="1:3">
       <c r="A271">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B271">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C271">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B272">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C272">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="273" spans="1:4">
@@ -4945,10 +4984,10 @@
         <v>4</v>
       </c>
       <c r="B273">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C273">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="274" spans="1:4">
@@ -4956,150 +4995,153 @@
         <v>4</v>
       </c>
       <c r="B274">
+        <v>32</v>
+      </c>
+      <c r="C274">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4">
+      <c r="A275">
+        <v>4</v>
+      </c>
+      <c r="B275">
+        <v>33</v>
+      </c>
+      <c r="C275">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4">
+      <c r="A276">
+        <v>4</v>
+      </c>
+      <c r="B276">
         <v>34</v>
       </c>
-      <c r="C274">
+      <c r="C276">
         <v>4</v>
       </c>
     </row>
-    <row r="276" spans="1:4">
-      <c r="A276" t="s">
+    <row r="278" spans="1:4">
+      <c r="A278" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="277" spans="1:4">
-      <c r="A277" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B277" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C277" s="1" t="s">
+    <row r="279" spans="1:4">
+      <c r="A279" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C279" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="D277" s="1" t="s">
+      <c r="D279" s="1" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="278" spans="1:4">
-      <c r="A278">
-        <v>1</v>
-      </c>
-      <c r="B278" t="s">
-        <v>255</v>
-      </c>
-      <c r="C278">
-        <v>1</v>
-      </c>
-      <c r="D278">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="279" spans="1:4">
-      <c r="A279">
-        <v>2</v>
-      </c>
-      <c r="B279" t="s">
-        <v>256</v>
-      </c>
-      <c r="C279">
-        <v>2</v>
-      </c>
-      <c r="D279">
-        <v>1</v>
       </c>
     </row>
     <row r="280" spans="1:4">
       <c r="A280">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B280" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C280">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D280">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:4">
       <c r="A281">
+        <v>2</v>
+      </c>
+      <c r="B281" t="s">
+        <v>256</v>
+      </c>
+      <c r="C281">
+        <v>2</v>
+      </c>
+      <c r="D281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4">
+      <c r="A282">
+        <v>3</v>
+      </c>
+      <c r="B282" t="s">
+        <v>257</v>
+      </c>
+      <c r="C282">
+        <v>1</v>
+      </c>
+      <c r="D282">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4">
+      <c r="A283">
         <v>4</v>
       </c>
-      <c r="B281" t="s">
+      <c r="B283" t="s">
         <v>258</v>
       </c>
-      <c r="C281">
+      <c r="C283">
+        <v>19</v>
+      </c>
+      <c r="D283">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4">
+      <c r="A284">
+        <v>5</v>
+      </c>
+      <c r="B284" t="s">
+        <v>295</v>
+      </c>
+      <c r="C284">
         <v>20</v>
       </c>
-      <c r="D281">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="283" spans="1:4">
-      <c r="A283" t="s">
+      <c r="D284">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4">
+      <c r="A286" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="284" spans="1:4">
-      <c r="A284" s="1" t="s">
+    <row r="287" spans="1:4">
+      <c r="A287" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B284" s="1" t="s">
+      <c r="B287" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C284" s="1" t="s">
+      <c r="C287" s="1" t="s">
         <v>251</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4">
-      <c r="A285">
-        <v>1</v>
-      </c>
-      <c r="B285">
-        <v>1</v>
-      </c>
-      <c r="C285">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="286" spans="1:4">
-      <c r="A286">
-        <v>1</v>
-      </c>
-      <c r="B286">
-        <v>2</v>
-      </c>
-      <c r="C286">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="287" spans="1:4">
-      <c r="A287">
-        <v>1</v>
-      </c>
-      <c r="B287">
-        <v>3</v>
-      </c>
-      <c r="C287">
-        <v>3</v>
       </c>
     </row>
     <row r="288" spans="1:4">
       <c r="A288">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B288">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C288">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B289">
         <v>2</v>
@@ -5110,32 +5152,32 @@
     </row>
     <row r="290" spans="1:3">
       <c r="A290">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B290">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C290">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="291" spans="1:3">
       <c r="A291">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B291">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C291">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B292">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C292">
         <v>2</v>
@@ -5143,13 +5185,13 @@
     </row>
     <row r="293" spans="1:3">
       <c r="A293">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B293">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C293">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="294" spans="1:3">
@@ -5157,10 +5199,10 @@
         <v>4</v>
       </c>
       <c r="B294">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C294">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="295" spans="1:3">
@@ -5179,64 +5221,64 @@
         <v>4</v>
       </c>
       <c r="B296">
+        <v>6</v>
+      </c>
+      <c r="C296">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297">
+        <v>5</v>
+      </c>
+      <c r="B297">
+        <v>6</v>
+      </c>
+      <c r="C297">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298">
+        <v>5</v>
+      </c>
+      <c r="B298">
+        <v>5</v>
+      </c>
+      <c r="C298">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299">
+        <v>5</v>
+      </c>
+      <c r="B299">
         <v>4</v>
       </c>
-      <c r="C296">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="298" spans="1:3">
-      <c r="A298" t="s">
+      <c r="C299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="299" spans="1:3">
-      <c r="A299" s="1" t="s">
+    <row r="302" spans="1:3">
+      <c r="A302" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B299" s="1" t="s">
+      <c r="B302" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="C299" s="1" t="s">
+      <c r="C302" s="1" t="s">
         <v>294</v>
-      </c>
-    </row>
-    <row r="300" spans="1:3">
-      <c r="A300">
-        <v>1</v>
-      </c>
-      <c r="B300">
-        <v>1</v>
-      </c>
-      <c r="C300">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="301" spans="1:3">
-      <c r="A301">
-        <v>2</v>
-      </c>
-      <c r="B301">
-        <v>1</v>
-      </c>
-      <c r="C301">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="302" spans="1:3">
-      <c r="A302">
-        <v>3</v>
-      </c>
-      <c r="B302">
-        <v>2</v>
-      </c>
-      <c r="C302">
-        <v>3</v>
       </c>
     </row>
     <row r="303" spans="1:3">
       <c r="A303">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B303">
         <v>1</v>
@@ -5247,258 +5289,313 @@
     </row>
     <row r="304" spans="1:3">
       <c r="A304">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B304">
         <v>2</v>
       </c>
       <c r="C304">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="A305">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B305">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C305">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="306" spans="1:3">
       <c r="A306">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B306">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C306">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="307" spans="1:3">
       <c r="A307">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B307">
+        <v>2</v>
+      </c>
+      <c r="C307">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3">
+      <c r="A308">
         <v>4</v>
       </c>
-      <c r="C307">
-        <v>3</v>
+      <c r="B308">
+        <v>1</v>
+      </c>
+      <c r="C308">
+        <v>2</v>
       </c>
     </row>
     <row r="309" spans="1:3">
-      <c r="A309" t="s">
-        <v>278</v>
+      <c r="A309">
+        <v>5</v>
+      </c>
+      <c r="B309">
+        <v>2</v>
+      </c>
+      <c r="C309">
+        <v>1</v>
       </c>
     </row>
     <row r="310" spans="1:3">
-      <c r="A310" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B310" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C310" s="1" t="s">
-        <v>259</v>
+      <c r="A310">
+        <v>6</v>
+      </c>
+      <c r="B310">
+        <v>1</v>
+      </c>
+      <c r="C310">
+        <v>1</v>
       </c>
     </row>
     <row r="311" spans="1:3">
       <c r="A311">
-        <v>1</v>
-      </c>
-      <c r="B311" t="s">
-        <v>262</v>
+        <v>7</v>
+      </c>
+      <c r="B311">
+        <v>4</v>
       </c>
       <c r="C311">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="312" spans="1:3">
       <c r="A312">
-        <v>2</v>
-      </c>
-      <c r="B312" t="s">
-        <v>263</v>
+        <v>8</v>
+      </c>
+      <c r="B312">
+        <v>5</v>
       </c>
       <c r="C312">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="313" spans="1:3">
-      <c r="A313">
-        <v>3</v>
-      </c>
-      <c r="B313" t="s">
-        <v>264</v>
-      </c>
-      <c r="C313">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="314" spans="1:3">
-      <c r="A314">
-        <v>4</v>
-      </c>
-      <c r="B314" t="s">
-        <v>265</v>
-      </c>
-      <c r="C314">
-        <v>2</v>
+      <c r="A314" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="315" spans="1:3">
-      <c r="A315">
-        <v>5</v>
-      </c>
-      <c r="B315" t="s">
-        <v>266</v>
-      </c>
-      <c r="C315">
-        <v>3</v>
+      <c r="A315" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="316" spans="1:3">
       <c r="A316">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B316" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C316">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="317" spans="1:3">
       <c r="A317">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B317" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="C317">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="318" spans="1:3">
       <c r="A318">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B318" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="C318">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3">
+      <c r="A319">
         <v>4</v>
       </c>
+      <c r="B319" t="s">
+        <v>265</v>
+      </c>
+      <c r="C319">
+        <v>2</v>
+      </c>
     </row>
     <row r="320" spans="1:3">
-      <c r="A320" t="s">
-        <v>279</v>
+      <c r="A320">
+        <v>5</v>
+      </c>
+      <c r="B320" t="s">
+        <v>266</v>
+      </c>
+      <c r="C320">
+        <v>3</v>
       </c>
     </row>
     <row r="321" spans="1:3">
-      <c r="A321" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B321" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C321" s="1" t="s">
-        <v>280</v>
+      <c r="A321">
+        <v>6</v>
+      </c>
+      <c r="B321" t="s">
+        <v>267</v>
+      </c>
+      <c r="C321">
+        <v>3</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B322" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C322">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="323" spans="1:3">
       <c r="A323">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B323" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C323">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="324" spans="1:3">
-      <c r="A324">
-        <v>3</v>
-      </c>
-      <c r="B324" t="s">
-        <v>272</v>
-      </c>
-      <c r="C324">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="325" spans="1:3">
-      <c r="A325">
-        <v>4</v>
-      </c>
-      <c r="B325" t="s">
-        <v>273</v>
-      </c>
-      <c r="C325">
-        <v>2</v>
+      <c r="A325" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="326" spans="1:3">
-      <c r="A326">
-        <v>5</v>
-      </c>
-      <c r="B326" t="s">
-        <v>274</v>
-      </c>
-      <c r="C326">
-        <v>3</v>
+      <c r="A326" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="327" spans="1:3">
       <c r="A327">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B327" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C327">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="328" spans="1:3">
       <c r="A328">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B328" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C328">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="329" spans="1:3">
       <c r="A329">
+        <v>3</v>
+      </c>
+      <c r="B329" t="s">
+        <v>272</v>
+      </c>
+      <c r="C329">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3">
+      <c r="A330">
+        <v>4</v>
+      </c>
+      <c r="B330" t="s">
+        <v>273</v>
+      </c>
+      <c r="C330">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3">
+      <c r="A331">
+        <v>5</v>
+      </c>
+      <c r="B331" t="s">
+        <v>274</v>
+      </c>
+      <c r="C331">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3">
+      <c r="A332">
+        <v>6</v>
+      </c>
+      <c r="B332" t="s">
+        <v>275</v>
+      </c>
+      <c r="C332">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3">
+      <c r="A333">
+        <v>7</v>
+      </c>
+      <c r="B333" t="s">
+        <v>276</v>
+      </c>
+      <c r="C333">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3">
+      <c r="A334">
         <v>8</v>
       </c>
-      <c r="B329" t="s">
+      <c r="B334" t="s">
         <v>277</v>
       </c>
-      <c r="C329">
+      <c r="C334">
         <v>4</v>
       </c>
     </row>
-    <row r="331" spans="1:3">
-      <c r="A331" t="s">
+    <row r="336" spans="1:3">
+      <c r="A336" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>